<commit_message>
ajout de fichier Modèles de compostage
</commit_message>
<xml_diff>
--- a/paramètres.xlsx
+++ b/paramètres.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\hravoaha\Desktop\process-development\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4F5DD37-0BCA-4B35-A71E-1F4FE88DCCDB}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99C5B530-91F7-446F-B438-16EBCF4FC11B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14380" windowHeight="4070" xr2:uid="{D303C9C8-6826-4A63-BBC4-6B6D232867EA}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14380" windowHeight="4070" activeTab="1" xr2:uid="{D303C9C8-6826-4A63-BBC4-6B6D232867EA}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
+    <sheet name="Feuil2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="116">
   <si>
     <t>Paramètres</t>
   </si>
@@ -367,6 +368,12 @@
   </si>
   <si>
     <t>kgDCO kg-1DCO</t>
+  </si>
+  <si>
+    <t>Chemin pour aller au dossier</t>
+  </si>
+  <si>
+    <t>/mnt/d/Users/hravoaha/Desktop/process-development</t>
   </si>
 </sst>
 </file>
@@ -732,8 +739,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6704EA7A-4173-4854-AD93-80A39703A317}">
   <dimension ref="A1:F45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="C46" sqref="C46"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1340,4 +1347,29 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6CC79754-8331-490C-971E-63A4A68A7F1A}">
+  <dimension ref="A1:A2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>115</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>